<commit_message>
update evidence format (A1-A6)
</commit_message>
<xml_diff>
--- a/DasRasyo/evidence.xlsx
+++ b/DasRasyo/evidence.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26130"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Fatih\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04EBEF7E-DE27-4160-B9F2-283E61F09781}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86111443-FE1F-417B-B428-B31C699F5C2E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="41">
   <si>
     <t>TxHash</t>
   </si>
@@ -79,24 +79,6 @@
     <t>nft id</t>
   </si>
   <si>
-    <t>tx hash on dest chain</t>
-  </si>
-  <si>
-    <t>dest chain id</t>
-  </si>
-  <si>
-    <t>tx hash on irisnet</t>
-  </si>
-  <si>
-    <t>ibc class on dest chain</t>
-  </si>
-  <si>
-    <t>class id you issued</t>
-  </si>
-  <si>
-    <t>nft id you minted</t>
-  </si>
-  <si>
     <t>TeamName</t>
   </si>
   <si>
@@ -119,30 +101,6 @@
   </si>
   <si>
     <t>Community</t>
-  </si>
-  <si>
-    <t>team name</t>
-  </si>
-  <si>
-    <t>addr1</t>
-  </si>
-  <si>
-    <t>addr2</t>
-  </si>
-  <si>
-    <t>addr3</t>
-  </si>
-  <si>
-    <t>addr4</t>
-  </si>
-  <si>
-    <t>addr5</t>
-  </si>
-  <si>
-    <t>discord#1234</t>
-  </si>
-  <si>
-    <t>set none if no community</t>
   </si>
   <si>
     <t>Conqueror</t>
@@ -601,10 +559,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:H3"/>
+  <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -621,80 +579,54 @@
   <sheetData>
     <row r="1" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>18</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="G2" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="H2" t="s">
         <v>26</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="G2" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="H2" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>33</v>
-      </c>
-      <c r="B3" t="s">
-        <v>34</v>
-      </c>
-      <c r="C3" t="s">
-        <v>35</v>
-      </c>
-      <c r="D3" t="s">
-        <v>36</v>
-      </c>
-      <c r="E3" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="F3" t="s">
-        <v>38</v>
-      </c>
-      <c r="G3" t="s">
-        <v>39</v>
-      </c>
-      <c r="H3" t="s">
-        <v>40</v>
       </c>
     </row>
   </sheetData>
@@ -1127,10 +1059,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1148,18 +1080,10 @@
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>41</v>
-      </c>
-      <c r="B3" t="s">
-        <v>42</v>
+        <v>27</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>28</v>
       </c>
     </row>
   </sheetData>
@@ -1400,10 +1324,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1425,35 +1349,24 @@
     </row>
     <row r="2" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>15</v>
+        <v>29</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>28</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>16</v>
+        <v>30</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>43</v>
+        <v>31</v>
       </c>
       <c r="B3" t="s">
-        <v>42</v>
+        <v>28</v>
       </c>
       <c r="C3" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>45</v>
-      </c>
-      <c r="B4" t="s">
-        <v>42</v>
-      </c>
-      <c r="C4" t="s">
-        <v>46</v>
+        <v>32</v>
       </c>
     </row>
   </sheetData>
@@ -1466,10 +1379,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1495,30 +1408,16 @@
     </row>
     <row r="2" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>14</v>
+        <v>33</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>34</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>47</v>
-      </c>
-      <c r="B3" t="s">
-        <v>48</v>
-      </c>
-      <c r="C3" t="s">
-        <v>44</v>
-      </c>
-      <c r="D3" t="s">
-        <v>49</v>
+        <v>35</v>
       </c>
     </row>
   </sheetData>
@@ -1531,10 +1430,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1560,30 +1459,16 @@
     </row>
     <row r="2" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>14</v>
+        <v>36</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>37</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>10</v>
+        <v>32</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>50</v>
-      </c>
-      <c r="B3" t="s">
-        <v>51</v>
-      </c>
-      <c r="C3" t="s">
-        <v>46</v>
-      </c>
-      <c r="D3" t="s">
-        <v>52</v>
+        <v>38</v>
       </c>
     </row>
   </sheetData>
@@ -1596,10 +1481,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1625,30 +1510,16 @@
     </row>
     <row r="2" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>9</v>
+        <v>39</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>34</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>53</v>
-      </c>
-      <c r="B3" t="s">
-        <v>48</v>
-      </c>
-      <c r="C3" t="s">
-        <v>44</v>
-      </c>
-      <c r="D3" t="s">
-        <v>49</v>
+        <v>35</v>
       </c>
     </row>
   </sheetData>
@@ -1661,10 +1532,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1691,30 +1562,16 @@
     </row>
     <row r="2" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>9</v>
+        <v>40</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>37</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>10</v>
+        <v>32</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>54</v>
-      </c>
-      <c r="B3" t="s">
-        <v>51</v>
-      </c>
-      <c r="C3" t="s">
-        <v>46</v>
-      </c>
-      <c r="D3" t="s">
-        <v>52</v>
+        <v>38</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update evidence with stage-2
</commit_message>
<xml_diff>
--- a/DasRasyo/evidence.xlsx
+++ b/DasRasyo/evidence.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Fatih\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86111443-FE1F-417B-B428-B31C699F5C2E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0C203EC-DF36-48D5-B956-0AC830B67AF1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="20" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Info" sheetId="1" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="72">
   <si>
     <t>TxHash</t>
   </si>
@@ -58,15 +58,6 @@
     <t>ChainID</t>
   </si>
   <si>
-    <t>tx hash on that chain</t>
-  </si>
-  <si>
-    <t>chain id</t>
-  </si>
-  <si>
-    <t>tx hash on that chain	chain id</t>
-  </si>
-  <si>
     <t>ClassID</t>
   </si>
   <si>
@@ -167,6 +158,108 @@
   </si>
   <si>
     <t>3F88138C5904C4D9BBC4E9EA7DC2B75CD536F4ECB3690EA64828F0BC0DAE8446</t>
+  </si>
+  <si>
+    <t>conquerornft4</t>
+  </si>
+  <si>
+    <t>ibc/1D373609288570B38A4135C434D2A6C1A5E0DEF54A4675A72C8D30375839C563</t>
+  </si>
+  <si>
+    <t>conquerornft7</t>
+  </si>
+  <si>
+    <t>ibc/C2A571FFEEB8F601062C378BE60D4329B47120DF8251ED7C0CE278A8B4EE3489</t>
+  </si>
+  <si>
+    <t>conquerornft9</t>
+  </si>
+  <si>
+    <t>ibc/B49D3C890B1A57060DF45F176285736987B53933B00DA306064C3F0914421DE1</t>
+  </si>
+  <si>
+    <t>DA223142375D4E567D9BE5D83BC28D27D4A7DB8F746696D02D0E968C9494CA9A</t>
+  </si>
+  <si>
+    <t>gon-irishub-1</t>
+  </si>
+  <si>
+    <t>81109473E36BDCCB70085EBEA9090E7D66A7C17716ACD83513D818F2B18981D6</t>
+  </si>
+  <si>
+    <t>elgafar-1</t>
+  </si>
+  <si>
+    <t>C8118DD31DC26A28ACCD5EBD1406579792C92495D891F24994F47FF2946C7E79</t>
+  </si>
+  <si>
+    <t>uptick_7000-2</t>
+  </si>
+  <si>
+    <t>816247F34A11DE50CE3079F60A6E45BB94156C7578DEFFE0495EA7B847DE23A7</t>
+  </si>
+  <si>
+    <t>C94F323BC5983CA9A704B656F2D8CFEFF40AB0A1589CE62AD013D01E540390E7</t>
+  </si>
+  <si>
+    <t>7C83AFF7E331670A150CC98AA5A6231E1AC4EA15AB10DE9D100B119E12508686</t>
+  </si>
+  <si>
+    <t>C276F95DFDF644652EADC03FBE6FEDE26BA701B3C83DE0A8EAEE537E5271E85D</t>
+  </si>
+  <si>
+    <t>C86419922802EA1F5CB7BABBF0F1D6FC3BE065D2669D5A193C5FA6122B3A6491</t>
+  </si>
+  <si>
+    <t>FF895E481A03FADE3861DC71AD8DDFD309AE678E604CC62E086A6E79DE817526</t>
+  </si>
+  <si>
+    <t>60F90B991BC64D5E091B6C88EB7084380C1409EC8948957D625C4CDC11602253</t>
+  </si>
+  <si>
+    <t>8538BF4B599196DF940D2AA96EE66A59034AB517830FC97E4EC192102D685A64</t>
+  </si>
+  <si>
+    <t>50BE7EA4B4F7AF0E835A9D17C3074BC4974A4B2EB75E6153FCBCBB58BB5CD2F7</t>
+  </si>
+  <si>
+    <t>63FD71730FBBDF261373C04A5AD6DE75E30F6284A714D26C5AE4D1D3EB24F600</t>
+  </si>
+  <si>
+    <t>3C35137CDC1D6B42165397838BF50FB1705FFD8D9E2FC42B21132DF5AFA56E29</t>
+  </si>
+  <si>
+    <t>DBF9F8BE0CD216B124C4AE7D55BEF16C0A32B90DE6322572D72A482CC2551DEC</t>
+  </si>
+  <si>
+    <t>6BB3548AF156C28133BE067FED824E1746C0C3BC9A2BD72734EC34EBEDC19E10</t>
+  </si>
+  <si>
+    <t>39AD65CC9A6C4FB6D99B66159077956319827AE6D8A7924A009D61F9775FD98D</t>
+  </si>
+  <si>
+    <t>7D71B41E93F1361F7E2C203F5D8C6227674F00570B7C7F6EE8166997E016AA12</t>
+  </si>
+  <si>
+    <t>53AC4B652F09A969EDEAA6E16773DAE6F14D7E35FEECFDC668D4C772F29330C6</t>
+  </si>
+  <si>
+    <t>F2493EA66B1FE67078D21164BFF141F1F07CE6DAE5BFBA0A8E5C2A324CCBA969</t>
+  </si>
+  <si>
+    <t>E03DF6F138DCCA9B3005CF41D88E872C978D88BBDE542D7A8BBC6D8514BCD42C</t>
+  </si>
+  <si>
+    <t>E7496681C51426427D06CE04F109A2E923FF8E81AD849BB4D3EF7C52D49E58F6</t>
+  </si>
+  <si>
+    <t>3CF9D94B8085BC0EA14E2B3675A4F855E95E3B70F662FCEAF494B9B6C3A95BE0</t>
+  </si>
+  <si>
+    <t>B9088CB806E1E73339938D23718859522EF03416B54D9825328FDA5F8CDDFF52</t>
+  </si>
+  <si>
+    <t>855563BC599A76DD20D5C7B46E3495249F42670B3DB0B7AA9AB6265C3C731E6D</t>
   </si>
 </sst>
 </file>
@@ -240,7 +333,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -252,6 +345,9 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -562,7 +658,7 @@
   <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -579,54 +675,54 @@
   <sheetData>
     <row r="1" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>15</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D2" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="E2" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="F2" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="G2" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="H2" t="s">
         <v>23</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="G2" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="H2" t="s">
-        <v>26</v>
       </c>
     </row>
   </sheetData>
@@ -651,18 +747,18 @@
   <sheetData>
     <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>7</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -672,390 +768,6 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
-  <sheetPr>
-    <outlinePr summaryBelow="0"/>
-  </sheetPr>
-  <dimension ref="A1:B2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="16" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.42578125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
-  <sheetPr>
-    <outlinePr summaryBelow="0"/>
-  </sheetPr>
-  <dimension ref="A1:B2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="16" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.42578125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
-  <sheetPr>
-    <outlinePr summaryBelow="0"/>
-  </sheetPr>
-  <dimension ref="A1:B2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="16" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.42578125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
-  <sheetPr>
-    <outlinePr summaryBelow="0"/>
-  </sheetPr>
-  <dimension ref="A1:B4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="16" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.42578125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
-  <sheetPr>
-    <outlinePr summaryBelow="0"/>
-  </sheetPr>
-  <dimension ref="A1:B4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="16" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.42578125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
-  <sheetPr>
-    <outlinePr summaryBelow="0"/>
-  </sheetPr>
-  <dimension ref="A1:B4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="16" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.42578125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
-  <sheetPr>
-    <outlinePr summaryBelow="0"/>
-  </sheetPr>
-  <dimension ref="A1:B4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="16" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.42578125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1100-000000000000}">
-  <sheetPr>
-    <outlinePr summaryBelow="0"/>
-  </sheetPr>
-  <dimension ref="A1:B4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="16" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.42578125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1200-000000000000}">
-  <sheetPr>
-    <outlinePr summaryBelow="0"/>
-  </sheetPr>
-  <dimension ref="A1:B4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="16" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.42578125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
@@ -1067,6 +779,454 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="16" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
+  <sheetPr>
+    <outlinePr summaryBelow="0"/>
+  </sheetPr>
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="16" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
+  <sheetPr>
+    <outlinePr summaryBelow="0"/>
+  </sheetPr>
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="16" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
+  <sheetPr>
+    <outlinePr summaryBelow="0"/>
+  </sheetPr>
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="16" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B3" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="B4" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="B5" t="s">
+        <v>47</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
+  <sheetPr>
+    <outlinePr summaryBelow="0"/>
+  </sheetPr>
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="16" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="B3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="B4" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="B5" t="s">
+        <v>49</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
+  <sheetPr>
+    <outlinePr summaryBelow="0"/>
+  </sheetPr>
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="16" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="B3" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="B4" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="B5" t="s">
+        <v>32</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
+  <sheetPr>
+    <outlinePr summaryBelow="0"/>
+  </sheetPr>
+  <dimension ref="A1:B4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="16" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="2"/>
+    </row>
+    <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="2"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1100-000000000000}">
+  <sheetPr>
+    <outlinePr summaryBelow="0"/>
+  </sheetPr>
+  <dimension ref="A1:B4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="16" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="2"/>
+    </row>
+    <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="2"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1200-000000000000}">
+  <sheetPr>
+    <outlinePr summaryBelow="0"/>
+  </sheetPr>
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="16" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="B3" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="B4" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="B5" t="s">
+        <v>35</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <sheetPr>
+    <outlinePr summaryBelow="0"/>
+  </sheetPr>
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
     <col min="1" max="2" width="17.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1075,15 +1235,15 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>28</v>
+        <v>24</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>25</v>
       </c>
     </row>
   </sheetData>
@@ -1098,7 +1258,9 @@
   </sheetPr>
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1116,66 +1278,94 @@
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>5</v>
+        <v>65</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="2"/>
+    </row>
+    <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="2"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1400-000000000000}">
+  <sheetPr>
+    <outlinePr summaryBelow="0"/>
+  </sheetPr>
+  <dimension ref="A1:B7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="16" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>6</v>
+        <v>67</v>
+      </c>
+      <c r="B3" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1400-000000000000}">
-  <sheetPr>
-    <outlinePr summaryBelow="0"/>
-  </sheetPr>
-  <dimension ref="A1:B4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="16" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.42578125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>6</v>
+        <v>68</v>
+      </c>
+      <c r="B4" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="B5" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="B6" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="B7" t="s">
+        <v>49</v>
       </c>
     </row>
   </sheetData>
@@ -1341,32 +1531,32 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>28</v>
+        <v>26</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>25</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B3" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="C3" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
     </row>
   </sheetData>
@@ -1397,10 +1587,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>3</v>
@@ -1408,16 +1598,16 @@
     </row>
     <row r="2" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>34</v>
+        <v>30</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>31</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
     </row>
   </sheetData>
@@ -1448,10 +1638,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>3</v>
@@ -1459,16 +1649,16 @@
     </row>
     <row r="2" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>37</v>
+        <v>33</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>34</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
   </sheetData>
@@ -1499,10 +1689,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>3</v>
@@ -1510,16 +1700,16 @@
     </row>
     <row r="2" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>34</v>
+        <v>36</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>31</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
     </row>
   </sheetData>
@@ -1534,7 +1724,7 @@
   </sheetPr>
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
@@ -1551,10 +1741,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>3</v>
@@ -1562,16 +1752,16 @@
     </row>
     <row r="2" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="B2" s="2" t="s">
         <v>37</v>
       </c>
+      <c r="B2" s="2" t="s">
+        <v>34</v>
+      </c>
       <c r="C2" s="2" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
   </sheetData>
@@ -1586,7 +1776,9 @@
   </sheetPr>
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1596,18 +1788,18 @@
   <sheetData>
     <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>7</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -1622,7 +1814,9 @@
   </sheetPr>
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1632,18 +1826,18 @@
   <sheetData>
     <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>8</v>
+        <v>4</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>10</v>
+        <v>39</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>38</v>
       </c>
     </row>
   </sheetData>

</xml_diff>